<commit_message>
exported graphs to pdf
</commit_message>
<xml_diff>
--- a/graphs/hyperparameters/Hyperparameter graphs.xlsx
+++ b/graphs/hyperparameters/Hyperparameter graphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OpenNLP" sheetId="3" r:id="rId1"/>
@@ -626,114 +626,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>OpenNLP!$G$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Filtered</c:v>
-                </c:pt>
-              </c:strCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>OpenNLP!$C$5:$C$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>OpenNLP!$G$5:$G$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>49.27</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>56.35</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>56.72</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>56.87</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>55.91</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>55.25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>54.56</c:v>
-                </c:pt>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-5CA0-4B5F-8191-4384CBA4CE81}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -746,7 +638,135 @@
         <c:smooth val="0"/>
         <c:axId val="427291440"/>
         <c:axId val="427292752"/>
-        <c:extLst/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>OpenNLP!$G$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Filtered</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>OpenNLP!$C$5:$C$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>OpenNLP!$G$5:$G$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>49.27</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>56.35</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>56.72</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>56.87</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>55.91</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>55.25</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>54.56</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-5CA0-4B5F-8191-4384CBA4CE81}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="427291440"/>
@@ -1037,7 +1057,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1503,156 +1523,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>OpenNLP!$G$32</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Filtered</c:v>
-                </c:pt>
-              </c:strCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>OpenNLP!$C$33:$C$46</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>200</c:v>
-                </c:pt>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>OpenNLP!$G$33:$G$46</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>55.83</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>56.27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>56.52</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>56.87</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>57.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>57.27</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>57.38</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>57.3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>57.3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>57.47</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>57.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>57.49</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>57.44</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>57.73</c:v>
-                </c:pt>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-1BF2-4848-A1A9-526F299EC110}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1665,7 +1535,177 @@
         <c:smooth val="0"/>
         <c:axId val="511839568"/>
         <c:axId val="511839896"/>
-        <c:extLst/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>OpenNLP!$G$32</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Filtered</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>OpenNLP!$C$33:$C$46</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>110</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>120</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>125</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>130</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>135</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>150</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>160</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>170</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>180</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>200</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>OpenNLP!$G$33:$G$46</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0">
+                        <c:v>55.83</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>56.27</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>56.52</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>56.87</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>57.16</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>57.27</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>57.38</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>57.3</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>57.3</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>57.47</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>57.5</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>57.49</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>57.44</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>57.73</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-1BF2-4848-A1A9-526F299EC110}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="511839568"/>
@@ -1966,7 +2006,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2396,144 +2436,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Spacy!$G$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Filtered</c:v>
-                </c:pt>
-              </c:strCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Spacy!$C$5:$C$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>120</c:v>
-                </c:pt>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Spacy!$G$5:$G$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>46.96</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>47.63</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>47.65</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>48.42</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>47.84</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>48.38</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>48.73</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>48.57</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48.26</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>48.37</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>49.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>49.09</c:v>
-                </c:pt>
-              </c:numCache>
-              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-B3B0-4412-A6D2-22FC3BC5BD58}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2546,7 +2448,165 @@
         <c:smooth val="0"/>
         <c:axId val="418370808"/>
         <c:axId val="418371464"/>
-        <c:extLst/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Spacy!$G$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Filtered</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Spacy!$C$5:$C$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>110</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>120</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Spacy!$G$5:$G$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>46.96</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>47.63</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>47.65</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>48.42</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>47.84</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>48.38</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>48.73</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>48.57</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>48.26</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>48.37</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>49.3</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>49.09</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000006-B3B0-4412-A6D2-22FC3BC5BD58}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="418370808"/>
@@ -2837,7 +2897,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3387,7 +3447,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -7473,8 +7533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="R50" sqref="R50"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7905,7 +7965,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -7914,8 +7974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8168,7 +8228,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -8177,7 +8237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -8268,7 +8328,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>